<commit_message>
File Area: Add support for .lrc files
</commit_message>
<xml_diff>
--- a/tests/files/wl_file_area/file_types/xlsx.xlsx
+++ b/tests/files/wl_file_area/file_types/xlsx.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\wl_tests_files\wl_file_area\file_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Wordless\tests\files\wl_file_area\file_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7F55BA-C9C4-4F9C-BDCF-5F40B0C144C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5B134F-B239-4E76-A6CD-28ADBC665406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{756ADEE8-81A0-48F6-B77E-381A0BA5C0D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -28,41 +36,41 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
+    <t>B2 &amp; C2</t>
+  </si>
+  <si>
+    <t>B3 &amp; B4</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
+    <t>D3</t>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
     <t>D2</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>B5</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>B2 &amp; C2</t>
-  </si>
-  <si>
-    <t>B3 &amp; B4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,12 +83,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,14 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -151,7 +147,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -163,7 +159,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -210,23 +206,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -262,23 +241,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,52 +392,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4B686C-0A0D-4E76-81F4-1A54C3FB4908}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
-        <v>9</v>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -484,81 +446,7 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:B4"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99B011F-06B2-42FF-9772-939C0DDAB83A}">
-  <dimension ref="C3:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="8.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="str">
-        <f>Sheet1!B2</f>
-        <v>B2 &amp; C2</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1" t="str">
-        <f>Sheet1!D2</f>
-        <v>D2</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="str">
-        <f>Sheet1!B3</f>
-        <v>B3 &amp; B4</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>Sheet1!C3</f>
-        <v>C3</v>
-      </c>
-      <c r="E4" s="2" t="str">
-        <f>Sheet1!D3</f>
-        <v>D3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
-      <c r="D5" s="2" t="str">
-        <f>Sheet1!C4</f>
-        <v>C4</v>
-      </c>
-      <c r="E5" s="2" t="str">
-        <f>Sheet1!D4</f>
-        <v>D4</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="str">
-        <f>Sheet1!B5</f>
-        <v>B5</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f>Sheet1!C5</f>
-        <v>C5</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <f>Sheet1!D5</f>
-        <v>D5</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:C5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
File Area: Fix support for .xlsx files
</commit_message>
<xml_diff>
--- a/tests/files/wl_file_area/file_types/xlsx.xlsx
+++ b/tests/files/wl_file_area/file_types/xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Wordless\tests\files\wl_file_area\file_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5B134F-B239-4E76-A6CD-28ADBC665406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6868C71E-8E6B-460E-8137-A3EDF13D1ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,15 +393,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -410,7 +417,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -421,7 +429,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -430,7 +439,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>